<commit_message>
increased R^2 to at least 0.6
</commit_message>
<xml_diff>
--- a/data/statistics/R-squared:RSME for temporal scales.xlsx
+++ b/data/statistics/R-squared:RSME for temporal scales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahhchu/Desktop/R/USCottonWeather/data/statistics/R-squared:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D733FA4-E447-B84B-8FDC-058984355398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D1822F-1F18-744C-A04F-28420A986947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15900" xr2:uid="{8B9E75E9-5AD8-4849-8BED-9D1D22815152}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15840" xr2:uid="{8B9E75E9-5AD8-4849-8BED-9D1D22815152}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Monthly </t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>RSME_Test</t>
+  </si>
+  <si>
+    <t>not 1988 + entire_scale</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAF8AD-6EAE-8B4E-B978-E5C198CD8E5C}">
-  <dimension ref="E5:J9"/>
+  <dimension ref="E5:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,7 +431,7 @@
     <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>7</v>
       </c>
@@ -447,85 +450,100 @@
       <c r="J5" t="s">
         <v>0</v>
       </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6">
-        <v>0.95548060000000001</v>
+        <v>0.95713199999999998</v>
       </c>
       <c r="G6">
-        <v>0.92558620000000003</v>
+        <v>0.95050230000000002</v>
       </c>
       <c r="H6">
-        <v>0.93867789999999995</v>
+        <v>0.95459760000000005</v>
       </c>
       <c r="I6">
-        <v>0.94550449999999997</v>
+        <v>0.95386249999999995</v>
       </c>
       <c r="J6">
-        <v>0.95847720000000003</v>
+        <v>0.95804310000000004</v>
+      </c>
+      <c r="L6">
+        <v>0.90412029999999999</v>
       </c>
     </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>0.29431760000000001</v>
+        <v>0.66669560000000005</v>
       </c>
       <c r="G7">
-        <v>0.11161409999999999</v>
+        <v>0.67541430000000002</v>
       </c>
       <c r="H7">
-        <v>0.16235140000000001</v>
+        <v>0.69006259999999997</v>
       </c>
       <c r="I7">
-        <v>0.26415539999999998</v>
+        <v>0.68827439999999995</v>
       </c>
       <c r="J7">
-        <v>0.29577310000000001</v>
+        <v>0.71332530000000005</v>
+      </c>
+      <c r="L7">
+        <v>0.58579820000000005</v>
       </c>
     </row>
-    <row r="8" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>8</v>
       </c>
       <c r="F8">
-        <v>1.0883910000000001</v>
+        <v>0.72757309999999997</v>
       </c>
       <c r="G8">
-        <v>1.1998789999999999</v>
+        <v>0.74498299999999995</v>
       </c>
       <c r="H8">
-        <v>1.16005</v>
+        <v>0.71458350000000004</v>
       </c>
       <c r="I8">
-        <v>1.1318569999999999</v>
+        <v>0.7199875</v>
       </c>
       <c r="J8">
-        <v>1.073868</v>
+        <v>0.69620930000000003</v>
+      </c>
+      <c r="L8">
+        <v>1.074109</v>
       </c>
     </row>
-    <row r="9" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>9</v>
       </c>
       <c r="F9">
-        <v>3.133397</v>
+        <v>1.9058470000000001</v>
       </c>
       <c r="G9">
-        <v>3.133397</v>
+        <v>1.8668720000000001</v>
       </c>
       <c r="H9">
-        <v>3.0075319999999999</v>
+        <v>1.8236129999999999</v>
       </c>
       <c r="I9">
-        <v>2.8425090000000002</v>
+        <v>1.8267960000000001</v>
       </c>
       <c r="J9">
-        <v>2.807833</v>
+        <v>1.757136</v>
+      </c>
+      <c r="L9">
+        <v>2.1296249999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed year and tested diff models for varimp
</commit_message>
<xml_diff>
--- a/data/statistics/R-squared:RSME for temporal scales.xlsx
+++ b/data/statistics/R-squared:RSME for temporal scales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahhchu/Desktop/R/USCottonWeather/data/statistics/R-squared:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D1822F-1F18-744C-A04F-28420A986947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EEF7E6-C536-6F46-9C8A-700BB30FD0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15840" xr2:uid="{8B9E75E9-5AD8-4849-8BED-9D1D22815152}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t xml:space="preserve">Monthly </t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>not 1988 + entire_scale</t>
+  </si>
+  <si>
+    <t>WITH YEAR</t>
+  </si>
+  <si>
+    <t>WITHOUT YEAR</t>
   </si>
 </sst>
 </file>
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAF8AD-6EAE-8B4E-B978-E5C198CD8E5C}">
-  <dimension ref="E5:L9"/>
+  <dimension ref="E4:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="L15:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,6 +437,11 @@
     <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="5" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>7</v>
@@ -544,6 +555,111 @@
       </c>
       <c r="L9">
         <v>2.1296249999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>0.93095170000000005</v>
+      </c>
+      <c r="G16">
+        <v>0.89611419999999997</v>
+      </c>
+      <c r="H16">
+        <v>0.91637990000000002</v>
+      </c>
+      <c r="I16">
+        <v>0.92126090000000005</v>
+      </c>
+      <c r="J16">
+        <v>0.9421235</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.26426240000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.1032163</v>
+      </c>
+      <c r="H17">
+        <v>0.13765759999999999</v>
+      </c>
+      <c r="I17">
+        <v>0.2008228</v>
+      </c>
+      <c r="J17">
+        <v>0.24345849999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>1.1101209999999999</v>
+      </c>
+      <c r="G18">
+        <v>1.2833749999999999</v>
+      </c>
+      <c r="H18">
+        <v>1.1861950000000001</v>
+      </c>
+      <c r="I18">
+        <v>1.158674</v>
+      </c>
+      <c r="J18">
+        <v>1.0812889999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>2.8240430000000001</v>
+      </c>
+      <c r="G19">
+        <v>3.1396310000000001</v>
+      </c>
+      <c r="H19">
+        <v>3.0429409999999999</v>
+      </c>
+      <c r="I19">
+        <v>2.9239259999999998</v>
+      </c>
+      <c r="J19">
+        <v>2.8593310000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added variable importance need to check
</commit_message>
<xml_diff>
--- a/data/statistics/R-squared:RSME for temporal scales.xlsx
+++ b/data/statistics/R-squared:RSME for temporal scales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahhchu/Desktop/R/USCottonWeather/data/statistics/R-squared:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EEF7E6-C536-6F46-9C8A-700BB30FD0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11C8E3-DD1A-E447-BD52-30E5EB14893D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15840" xr2:uid="{8B9E75E9-5AD8-4849-8BED-9D1D22815152}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{8B9E75E9-5AD8-4849-8BED-9D1D22815152}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t xml:space="preserve">Monthly </t>
   </si>
@@ -73,6 +73,60 @@
   </si>
   <si>
     <t>WITHOUT YEAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">              variable    Overall</t>
+  </si>
+  <si>
+    <t>1       srad_sum_April 6.79172717</t>
+  </si>
+  <si>
+    <t>2     tmax_mean_August 5.51094814</t>
+  </si>
+  <si>
+    <t>3       tamp_mean_July 5.37070104</t>
+  </si>
+  <si>
+    <t>4  dayl_mean_September 5.24681141</t>
+  </si>
+  <si>
+    <t>5     gdd_sum_November 4.87230151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                       variable    Overall</t>
+  </si>
+  <si>
+    <t>1                              gdd_sum_November  4.4389873</t>
+  </si>
+  <si>
+    <t>2                                tamp_mean_July  4.2799157</t>
+  </si>
+  <si>
+    <t>3                            gdd_mean_June_July  4.1157730</t>
+  </si>
+  <si>
+    <t>4                        gdd_mean_growingseason  3.9875056</t>
+  </si>
+  <si>
+    <t>5                            srad_sum_September  3.8805598</t>
+  </si>
+  <si>
+    <t>All Temporal Scale:</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>tamp_mean_July</t>
+  </si>
+  <si>
+    <t>gdd_sum_November</t>
+  </si>
+  <si>
+    <t>Variable  Importance using vip()</t>
   </si>
 </sst>
 </file>
@@ -424,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAF8AD-6EAE-8B4E-B978-E5C198CD8E5C}">
-  <dimension ref="E4:L19"/>
+  <dimension ref="E4:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="L15:M19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,7 +656,7 @@
         <v>0.9421235</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>1</v>
       </c>
@@ -622,7 +676,7 @@
         <v>0.24345849999999999</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>8</v>
       </c>
@@ -642,7 +696,7 @@
         <v>1.0812889999999999</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>9</v>
       </c>
@@ -660,6 +714,76 @@
       </c>
       <c r="J19">
         <v>2.8593310000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
found weather variables that are common across different temporal scale and varImp()/vip() functions
</commit_message>
<xml_diff>
--- a/data/statistics/R-squared:RSME for temporal scales.xlsx
+++ b/data/statistics/R-squared:RSME for temporal scales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahhchu/Desktop/R/USCottonWeather/data/statistics/R-squared:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11C8E3-DD1A-E447-BD52-30E5EB14893D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A002A95E-35D1-2B4D-84CB-A568205322D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{8B9E75E9-5AD8-4849-8BED-9D1D22815152}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t xml:space="preserve">Monthly </t>
   </si>
@@ -75,58 +75,7 @@
     <t>WITHOUT YEAR</t>
   </si>
   <si>
-    <t xml:space="preserve">Monthly: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">              variable    Overall</t>
-  </si>
-  <si>
-    <t>1       srad_sum_April 6.79172717</t>
-  </si>
-  <si>
-    <t>2     tmax_mean_August 5.51094814</t>
-  </si>
-  <si>
-    <t>3       tamp_mean_July 5.37070104</t>
-  </si>
-  <si>
-    <t>4  dayl_mean_September 5.24681141</t>
-  </si>
-  <si>
-    <t>5     gdd_sum_November 4.87230151</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                       variable    Overall</t>
-  </si>
-  <si>
-    <t>1                              gdd_sum_November  4.4389873</t>
-  </si>
-  <si>
-    <t>2                                tamp_mean_July  4.2799157</t>
-  </si>
-  <si>
-    <t>3                            gdd_mean_June_July  4.1157730</t>
-  </si>
-  <si>
-    <t>4                        gdd_mean_growingseason  3.9875056</t>
-  </si>
-  <si>
-    <t>5                            srad_sum_September  3.8805598</t>
-  </si>
-  <si>
-    <t>All Temporal Scale:</t>
-  </si>
-  <si>
-    <t>Same</t>
-  </si>
-  <si>
-    <t>tamp_mean_July</t>
-  </si>
-  <si>
-    <t>gdd_sum_November</t>
-  </si>
-  <si>
-    <t>Variable  Importance using vip()</t>
+    <t># mtry = 90, trees = 35)</t>
   </si>
 </sst>
 </file>
@@ -478,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAF8AD-6EAE-8B4E-B978-E5C198CD8E5C}">
-  <dimension ref="E4:M31"/>
+  <dimension ref="E2:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,6 +440,11 @@
     <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="4" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>11</v>
@@ -656,7 +610,7 @@
         <v>0.9421235</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>1</v>
       </c>
@@ -676,7 +630,7 @@
         <v>0.24345849999999999</v>
       </c>
     </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>8</v>
       </c>
@@ -696,7 +650,7 @@
         <v>1.0812889999999999</v>
       </c>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>9</v>
       </c>
@@ -714,76 +668,6 @@
       </c>
       <c r="J19">
         <v>2.8593310000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" t="s">
-        <v>20</v>
-      </c>
-      <c r="M26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="s">
-        <v>21</v>
-      </c>
-      <c r="M27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E28" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-      <c r="M28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>